<commit_message>
Modified The Hive Tracker
</commit_message>
<xml_diff>
--- a/The Hive Tracker.xlsx
+++ b/The Hive Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EA7E8D-102A-401B-A6B7-34B629EBD2EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386BDE5A-3997-4E53-8452-BF1DC59DD933}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1717,7 +1717,7 @@
   <dimension ref="A1:BP21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -2984,7 +2984,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="21">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="F12" s="22">
         <v>44696</v>
@@ -3474,7 +3474,7 @@
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="21">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F14" s="22">
         <v>44696</v>
@@ -3964,7 +3964,7 @@
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="21">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="F16" s="22">
         <v>44696</v>
@@ -4209,7 +4209,7 @@
       </c>
       <c r="D17" s="20"/>
       <c r="E17" s="21">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="F17" s="22">
         <v>44696</v>
@@ -4958,34 +4958,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="22a266b9fa9a230c5a512669d8b298c3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eddc33fff6b14141ee5c74a0d29ea6a1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5261,27 +5233,35 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75C87518-DD8E-42CD-8DAC-291A323E849B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5300,4 +5280,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>